<commit_message>
fix: ready to present
</commit_message>
<xml_diff>
--- a/angkost_result.xlsx
+++ b/angkost_result.xlsx
@@ -11,6 +11,7 @@
     <sheet name="HIGH_PRICE (ANGKOST)" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="LOW_SCORE (ANGKOST)" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="HIGH_SCORE (ANGKOST)" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="RECOMMENDATION (ANGKOST)" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -417,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,6 +484,34 @@
       </c>
       <c r="F2" t="n">
         <v>5002.900000000001</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1414556557</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Blinqshop Baju Tidur Piyama Motid Aurel</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Rp27.900</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://www.tokopedia.com/blinqshop/blinqshop-baju-tidur-piyama-motid-aurel-dst-putih?extParam=ivf%3Dfalse%26src%3Dsearch</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>1048.8</v>
       </c>
     </row>
   </sheetData>
@@ -497,7 +526,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -539,30 +568,58 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>545554122</v>
+        <v>1862123531</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Logitech Pebble M350 Mouse Wireless Bluetooth Slim Silent - Graphite</t>
+          <t>Logitech G304 Lightspeed Wireless Gaming Mouse - Logitech G-304</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Rp282.000</t>
+          <t>Rp498.000</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://www.tokopedia.com/logitech/logitech-pebble-m350-mouse-wireless-bluetooth-slim-silent-graphite?extParam=ivf%3Dfalse%26src%3Dsearch%26whid%3D5931369</t>
+          <t>https://www.tokopedia.com/duniacom-srv/logitech-g304-lightspeed-wireless-gaming-mouse-logitech-g-304-putih?extParam=ivf%3Dfalse%26src%3Dsearch</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>25847.5</v>
+        <v>4055</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1722207942</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Baju Tidur Wanita Setelan Panjang / Piyama Set Kimono</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Rp118.340</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>4.7</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://www.tokopedia.com/twinolshop-2/baju-tidur-wanita-setelan-panjang-piyama-set-kimono-pink-leaf?extParam=ivf%3Dfalse%26src%3Dsearch</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>4107.8</v>
       </c>
     </row>
   </sheetData>
@@ -577,7 +634,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -619,30 +676,58 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>424159251</v>
+        <v>1862123531</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Mouse USB Logitech M90</t>
+          <t>Logitech G304 Lightspeed Wireless Gaming Mouse - Logitech G-304</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Rp43.000</t>
+          <t>Rp498.000</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>5.0</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>https://www.tokopedia.com/duniacom-srv/logitech-g304-lightspeed-wireless-gaming-mouse-logitech-g-304-putih?extParam=ivf%3Dfalse%26src%3Dsearch</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>4055</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1977206481</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Lingerie Sexy Outer+Dress Transparan Piyama Baju Tidur Kimono Lr11</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Rp92.000</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>4.9</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>https://www.tokopedia.com/dbclick/mouse-usb-logitech-m90?extParam=ivf%3Dfalse%26src%3Dsearch%26whid%3D13037795</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>5002.900000000001</v>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://www.tokopedia.com/officialbianglalaid/lingerie-sexy-outer-dress-transparan-piyama-baju-tidur-kimono-lr11-merah?extParam=ivf%3Dfalse%26src%3Dsearch</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>955.5000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -657,7 +742,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -722,7 +807,143 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>173616.8</v>
+        <v>173626.6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1722207942</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Baju Tidur Wanita Setelan Panjang / Piyama Set Kimono</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Rp118.340</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>4.7</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://www.tokopedia.com/twinolshop-2/baju-tidur-wanita-setelan-panjang-piyama-set-kimono-pink-leaf?extParam=ivf%3Dfalse%26src%3Dsearch</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>4107.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <tabColor rgb="00FFC400"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Id Produk</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Nama Produk</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Harga Produk</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Bintang Produk</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Link Produk</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Skor Produk (Rekomendasi)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1862123531</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Logitech G304 Lightspeed Wireless Gaming Mouse - Logitech G-304</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Rp498.000</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>https://www.tokopedia.com/duniacom-srv/logitech-g304-lightspeed-wireless-gaming-mouse-logitech-g-304-putih?extParam=ivf%3Dfalse%26src%3Dsearch</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>6.973817219257057</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1977206481</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Lingerie Sexy Outer+Dress Transparan Piyama Baju Tidur Kimono Lr11</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Rp92.000</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>4.9</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://www.tokopedia.com/officialbianglalaid/lingerie-sexy-outer-dress-transparan-piyama-baju-tidur-kimono-lr11-merah?extParam=ivf%3Dfalse%26src%3Dsearch</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>3.482186883868269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>